<commit_message>
Generate cylindrical lens gds
</commit_message>
<xml_diff>
--- a/data/lens_discretization.xlsx
+++ b/data/lens_discretization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vahlin\Documents\Exjobb\Vera simulations\Fresnel lens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CHIT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1B58B7-23A5-4093-9AC5-E58A3C4BA25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2192B45-6578-44FD-AE88-625803AFC241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2674D905-5BF6-41A4-84E9-E0FBCC1957D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2674D905-5BF6-41A4-84E9-E0FBCC1957D6}"/>
   </bookViews>
   <sheets>
     <sheet name="x-pol" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M56" sqref="M56"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>